<commit_message>
update some rules, ready to finish refresh() tomorrow
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D3FE9-E0A4-4E6F-9CCD-52D298B253B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358C581F-9427-47EE-A3E0-7D08F9826F33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -222,7 +222,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -332,6 +332,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,13 +351,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -647,17 +647,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -944,7 +944,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF40BAA-8A38-4EF9-A863-ECFFAD2B3CB6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -962,16 +962,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1122,94 +1122,94 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1217,7 +1217,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1240,15 +1240,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1522,8 +1522,8 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
@@ -1534,7 +1534,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="11"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
@@ -1555,7 +1555,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1575,20 +1575,20 @@
     <col min="4" max="4" width="10.375" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="5">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1625,7 +1625,7 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="5">
         <v>120</v>
       </c>
       <c r="E3" s="3">
@@ -1640,7 +1640,7 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1649,7 +1649,7 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>100</v>
       </c>
       <c r="E4" s="3">
@@ -1664,7 +1664,7 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1673,7 +1673,7 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <v>100</v>
       </c>
       <c r="E5" s="3">
@@ -1688,7 +1688,7 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1697,7 +1697,7 @@
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>90</v>
       </c>
       <c r="E6" s="3">
@@ -1712,7 +1712,7 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1721,7 +1721,7 @@
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>80</v>
       </c>
       <c r="E7" s="3">
@@ -1741,6 +1741,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish new move model so players can move(ignore obstacle)
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358C581F-9427-47EE-A3E0-7D08F9826F33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729BB0B5-ADDD-46AB-B3C6-A254FE5F29D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1629,7 @@
         <v>120</v>
       </c>
       <c r="E3" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
@@ -1653,7 +1653,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
@@ -1677,7 +1677,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="3">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -1701,7 +1701,7 @@
         <v>90</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
@@ -1725,7 +1725,7 @@
         <v>80</v>
       </c>
       <c r="E7" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
start to finish shoot part, still need to debug
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729BB0B5-ADDD-46AB-B3C6-A254FE5F29D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7890B091-6CC3-47EA-AF3F-ADB739961446}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,14 @@
   </si>
   <si>
     <t>减小武器发出的声音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视距</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视角</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -634,7 +642,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="3">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -953,7 +961,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1234,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1561,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1573,13 +1581,15 @@
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="11.75" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
@@ -1589,9 +1599,11 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1605,17 +1617,23 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -1628,18 +1646,24 @@
       <c r="D3" s="5">
         <v>120</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
+        <v>200</v>
+      </c>
+      <c r="F3" s="5">
+        <v>124</v>
+      </c>
+      <c r="G3" s="3">
         <v>1.8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3">
+      <c r="I3" s="3">
         <v>1.5</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1652,18 +1676,24 @@
       <c r="D4" s="5">
         <v>100</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
+        <v>200</v>
+      </c>
+      <c r="F4" s="5">
+        <v>124</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1676,18 +1706,24 @@
       <c r="D5" s="5">
         <v>100</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
+        <v>200</v>
+      </c>
+      <c r="F5" s="5">
+        <v>124</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3">
+      <c r="I5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1700,18 +1736,24 @@
       <c r="D6" s="5">
         <v>90</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
+        <v>200</v>
+      </c>
+      <c r="F6" s="5">
+        <v>124</v>
+      </c>
+      <c r="G6" s="3">
         <v>1.2</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -1724,20 +1766,26 @@
       <c r="D7" s="5">
         <v>80</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
+        <v>250</v>
+      </c>
+      <c r="F7" s="5">
+        <v>115</v>
+      </c>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3">
+      <c r="I7" s="3">
         <v>1.5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
debug for the circle part, ready to test with platform
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48E5C01-78C9-4C9D-8DF7-239689A2D761}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137E2693-4A30-476D-9519-3F5EC4B5CF18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -401,6 +401,12 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,12 +417,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -715,17 +715,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1030,16 +1030,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1308,15 +1308,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1631,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1650,17 +1650,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1872,18 +1872,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1940,7 +1940,7 @@
         <f>1000 * F3</f>
         <v>750</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="11">
         <f>(1000-G3)/D3</f>
         <v>1.25</v>
       </c>
@@ -1948,7 +1948,7 @@
         <f>(B3+C3+D3)</f>
         <v>600</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="10">
         <f>I3</f>
         <v>600</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>200</v>
       </c>
       <c r="D4" s="3">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E4" s="8">
         <v>0.75</v>
@@ -1976,17 +1976,17 @@
         <f>G3*F4</f>
         <v>450</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="11">
         <f>(G3-G4)/D4</f>
-        <v>1.5</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="I4" s="3">
         <f>(C4+D4)</f>
-        <v>400</v>
-      </c>
-      <c r="J4" s="14">
+        <v>380</v>
+      </c>
+      <c r="J4" s="10">
         <f>I4+J3</f>
-        <v>1000</v>
+        <v>980</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
         <v>200</v>
       </c>
       <c r="D5" s="3">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
@@ -2012,17 +2012,17 @@
         <f t="shared" ref="G5:G11" si="0">G4*F5</f>
         <v>225</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="11">
         <f t="shared" ref="H5:H11" si="1">(G4-G5)/D5</f>
-        <v>1.125</v>
+        <v>1.40625</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" ref="I5:I11" si="2">(C5+D5)</f>
-        <v>400</v>
-      </c>
-      <c r="J5" s="14">
+        <v>360</v>
+      </c>
+      <c r="J5" s="10">
         <f t="shared" ref="J5:J11" si="3">I5+J4</f>
-        <v>1400</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
         <v>200</v>
       </c>
       <c r="D6" s="3">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="E6" s="8">
         <v>1.25</v>
@@ -2048,17 +2048,17 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="11">
         <f t="shared" si="1"/>
-        <v>0.5625</v>
+        <v>0.8035714285714286</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J6" s="14">
+        <v>340</v>
+      </c>
+      <c r="J6" s="10">
         <f t="shared" si="3"/>
-        <v>1800</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="3">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="E7" s="8">
         <v>1.5</v>
@@ -2084,17 +2084,17 @@
         <f t="shared" si="0"/>
         <v>56.25</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <f t="shared" si="1"/>
-        <v>0.28125</v>
+        <v>0.46875</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J7" s="14">
+        <v>320</v>
+      </c>
+      <c r="J7" s="10">
         <f t="shared" si="3"/>
-        <v>2200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2108,7 +2108,7 @@
         <v>200</v>
       </c>
       <c r="D8" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E8" s="8">
         <v>2</v>
@@ -2120,17 +2120,17 @@
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="11">
         <f t="shared" si="1"/>
-        <v>0.140625</v>
+        <v>0.28125</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J8" s="14">
+        <v>300</v>
+      </c>
+      <c r="J8" s="10">
         <f t="shared" si="3"/>
-        <v>2600</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2144,7 +2144,7 @@
         <v>200</v>
       </c>
       <c r="D9" s="3">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="E9" s="8">
         <v>3</v>
@@ -2156,17 +2156,17 @@
         <f t="shared" si="0"/>
         <v>14.0625</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="11">
         <f t="shared" si="1"/>
-        <v>7.03125E-2</v>
+        <v>0.17578125</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J9" s="14">
+        <v>280</v>
+      </c>
+      <c r="J9" s="10">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2180,7 +2180,7 @@
         <v>200</v>
       </c>
       <c r="D10" s="3">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="E10" s="8">
         <v>5</v>
@@ -2192,17 +2192,17 @@
         <f t="shared" si="0"/>
         <v>7.03125</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="11">
         <f t="shared" si="1"/>
-        <v>3.515625E-2</v>
+        <v>0.1171875</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J10" s="14">
+        <v>260</v>
+      </c>
+      <c r="J10" s="10">
         <f t="shared" si="3"/>
-        <v>3400</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
         <v>200</v>
       </c>
       <c r="D11" s="3">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="E11" s="8">
         <v>10</v>
@@ -2228,17 +2228,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="11">
         <f t="shared" si="1"/>
-        <v>3.515625E-2</v>
+        <v>0.17578125</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="J11" s="14">
+        <v>240</v>
+      </c>
+      <c r="J11" s="10">
         <f t="shared" si="3"/>
-        <v>3800</v>
+        <v>3080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish sound part basically
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137E2693-4A30-476D-9519-3F5EC4B5CF18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B48CF92-8137-4BF1-BC1F-B37B90279B65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="道具" sheetId="3" r:id="rId3"/>
     <sheet name="角色" sheetId="1" r:id="rId4"/>
     <sheet name="毒圈" sheetId="5" r:id="rId5"/>
+    <sheet name="声音" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,6 +268,70 @@
   </si>
   <si>
     <t>阶段帧数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>声音数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脚步声</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无线电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枪声</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RADIO_VOICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOOTSTEP_SOUND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUN_SOUND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传播距离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>声速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动三步的第二步产生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点对点通信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用武器攻击时发出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆炸声</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOM_SOUND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆炸物爆炸时发出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -376,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -417,6 +482,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1632,7 +1700,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection sqref="A1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2249,4 +2317,149 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22578DC-6594-4E6E-A10D-A4570B4B155F}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="22.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="5">
+        <v>500</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3000</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="5">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5">
+        <v>100</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="5">
+        <v>100</v>
+      </c>
+      <c r="E5" s="5">
+        <v>300</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="5">
+        <v>200</v>
+      </c>
+      <c r="E6" s="5">
+        <v>600</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix move bug, finish air drop initialize part
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDE7DD1-E8A6-4A84-AFC9-19384FC2D4A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A916F3E-9AAD-481B-8524-E8536AA7249D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="127">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -460,10 +460,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>散角</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>无视护甲</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -517,6 +513,26 @@
   </si>
   <si>
     <t>护甲减伤曲线的参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绝缘服</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INSULATED_CLOTHING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只能用于抵挡毒伤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>散角参数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -636,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -667,6 +683,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,12 +696,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -968,7 +981,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -982,18 +995,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1012,7 +1025,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>22</v>
@@ -1059,6 +1072,7 @@
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
+        <f>IF(ISBLANK(B4),"",A3+1)</f>
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1089,6 +1103,7 @@
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
+        <f t="shared" ref="A5:A15" si="0">IF(ISBLANK(B5),"",A4+1)</f>
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1119,6 +1134,7 @@
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1149,6 +1165,7 @@
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1179,6 +1196,7 @@
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1209,6 +1227,7 @@
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1239,6 +1258,7 @@
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1269,6 +1289,7 @@
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1299,13 +1320,14 @@
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1326,12 +1348,13 @@
         <v>25</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>10</v>
+      <c r="A13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1344,8 +1367,9 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>11</v>
+      <c r="A14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1358,8 +1382,9 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>12</v>
+      <c r="A15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1457,26 +1482,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF40BAA-8A38-4EF9-A863-ECFFAD2B3CB6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1506,7 +1532,8 @@
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>13</v>
+        <f>COUNT(武器!A3:A25)</f>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>31</v>
@@ -1517,7 +1544,7 @@
       <c r="D3" s="3">
         <v>100</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="12">
         <v>0.15</v>
       </c>
       <c r="F3" s="3">
@@ -1532,7 +1559,8 @@
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>14</v>
+        <f>IF(ISBLANK(B4),"",A3+1)</f>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>71</v>
@@ -1543,7 +1571,7 @@
       <c r="D4" s="3">
         <v>150</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="12">
         <v>0.25</v>
       </c>
       <c r="F4" s="3">
@@ -1558,7 +1586,8 @@
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>15</v>
+        <f t="shared" ref="A5:A8" si="0">IF(ISBLANK(B5),"",A4+1)</f>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>72</v>
@@ -1569,7 +1598,7 @@
       <c r="D5" s="3">
         <v>200</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="12">
         <v>0.3</v>
       </c>
       <c r="F5" s="3">
@@ -1584,36 +1613,53 @@
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="3">
+        <v>100</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>17</v>
+      <c r="A7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>18</v>
+      <c r="A8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1752,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74A35FB-70A1-4854-8376-A9BDA6B66FB9}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1767,16 +1813,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1795,7 +1841,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>37</v>
@@ -1806,7 +1852,8 @@
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>21</v>
+        <f>COUNT(防具!A3:A10) + COUNT(武器!A3:A20)</f>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>35</v>
@@ -1832,7 +1879,8 @@
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>22</v>
+        <f>IF(ISBLANK(B4),"",A3+1)</f>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>91</v>
@@ -1858,7 +1906,8 @@
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>23</v>
+        <f t="shared" ref="A5:A13" si="0">IF(ISBLANK(B5),"",A4+1)</f>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>93</v>
@@ -1884,7 +1933,8 @@
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>98</v>
@@ -1909,8 +1959,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>25</v>
+      <c r="A7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1921,8 +1972,9 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>26</v>
+      <c r="A8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1933,8 +1985,9 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>27</v>
+      <c r="A9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1945,8 +1998,9 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>28</v>
+      <c r="A10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1957,8 +2011,9 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>29</v>
+      <c r="A11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1969,8 +2024,9 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>30</v>
+      <c r="A12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1981,8 +2037,9 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>31</v>
+      <c r="A13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2137,7 +2194,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2155,18 +2212,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2346,399 +2403,431 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.375" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="8.25" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="11.75" customWidth="1"/>
-    <col min="10" max="10" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="7.125" customWidth="1"/>
+    <col min="3" max="3" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="11" max="11" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>0</v>
       </c>
       <c r="B3" s="9">
-        <v>200</v>
-      </c>
-      <c r="C3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="9">
         <v>200</v>
       </c>
       <c r="D3" s="3">
         <v>200</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="8">
         <v>0.5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>0.75</v>
       </c>
-      <c r="G3" s="8">
-        <f>1000 * F3</f>
+      <c r="H3" s="8">
+        <f>1000 * G3</f>
         <v>750</v>
       </c>
-      <c r="H3" s="10">
-        <f>(1000-G3)/D3</f>
+      <c r="I3" s="10">
+        <f>(1000-H3)/E3</f>
         <v>1.25</v>
       </c>
-      <c r="I3" s="9">
-        <f>(B3+C3+D3)</f>
+      <c r="J3" s="9">
+        <f>(C3+D3+E3)</f>
         <v>600</v>
       </c>
-      <c r="J3" s="9">
-        <f>I3</f>
+      <c r="K3" s="9">
+        <f>J3</f>
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9">
+        <v>500</v>
+      </c>
+      <c r="C4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>200</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>180</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="8">
         <v>0.75</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
-        <f>G3*F4</f>
+      <c r="H4" s="8">
+        <f>H3*G4</f>
         <v>450</v>
       </c>
-      <c r="H4" s="10">
-        <f>(G3-G4)/D4</f>
+      <c r="I4" s="10">
+        <f>(H3-H4)/E4</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I4" s="9">
-        <f>(C4+D4)</f>
+      <c r="J4" s="9">
+        <f>(D4+E4)</f>
         <v>380</v>
       </c>
-      <c r="J4" s="9">
-        <f>I4+J3</f>
+      <c r="K4" s="9">
+        <f>J4+K3</f>
         <v>980</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9">
+        <v>250</v>
+      </c>
+      <c r="C5" s="9">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>200</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>160</v>
       </c>
-      <c r="E5" s="8">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>0.5</v>
       </c>
-      <c r="G5" s="8">
-        <f t="shared" ref="G5:G11" si="0">G4*F5</f>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:H11" si="0">H4*G5</f>
         <v>225</v>
       </c>
-      <c r="H5" s="10">
-        <f t="shared" ref="H5:H11" si="1">(G4-G5)/D5</f>
+      <c r="I5" s="10">
+        <f t="shared" ref="I5:I11" si="1">(H4-H5)/E5</f>
         <v>1.40625</v>
       </c>
-      <c r="I5" s="9">
-        <f t="shared" ref="I5:I11" si="2">(C5+D5)</f>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J11" si="2">(D5+E5)</f>
         <v>360</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" ref="J5:J11" si="3">I5+J4</f>
+      <c r="K5" s="9">
+        <f t="shared" ref="K5:K11" si="3">J5+K4</f>
         <v>1340</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="9">
+        <v>125</v>
+      </c>
+      <c r="C6" s="9">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>200</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>140</v>
       </c>
-      <c r="E6" s="8">
+      <c r="F6" s="8">
         <v>1.25</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>0.5</v>
       </c>
-      <c r="G6" s="8">
+      <c r="H6" s="8">
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="10">
         <f t="shared" si="1"/>
         <v>0.8035714285714286</v>
       </c>
-      <c r="I6" s="9">
+      <c r="J6" s="9">
         <f t="shared" si="2"/>
         <v>340</v>
       </c>
-      <c r="J6" s="9">
+      <c r="K6" s="9">
         <f t="shared" si="3"/>
         <v>1680</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>4</v>
       </c>
       <c r="B7" s="9">
+        <v>63</v>
+      </c>
+      <c r="C7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>200</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>120</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F7" s="8">
         <v>1.5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>0.5</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="8">
         <f t="shared" si="0"/>
         <v>56.25</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="10">
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
-      <c r="I7" s="9">
+      <c r="J7" s="9">
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
-      <c r="J7" s="9">
+      <c r="K7" s="9">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="9">
+        <v>50</v>
+      </c>
+      <c r="C8" s="9">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>200</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>0.5</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <f t="shared" si="1"/>
         <v>0.28125</v>
       </c>
-      <c r="I8" s="9">
+      <c r="J8" s="9">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="J8" s="9">
+      <c r="K8" s="9">
         <f t="shared" si="3"/>
         <v>2300</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>6</v>
       </c>
       <c r="B9" s="9">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>200</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>80</v>
       </c>
-      <c r="E9" s="8">
+      <c r="F9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H9" s="8">
         <f t="shared" si="0"/>
         <v>14.0625</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="10">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="I9" s="9">
+      <c r="J9" s="9">
         <f t="shared" si="2"/>
         <v>280</v>
       </c>
-      <c r="J9" s="9">
+      <c r="K9" s="9">
         <f t="shared" si="3"/>
         <v>2580</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>7</v>
       </c>
       <c r="B10" s="9">
+        <v>50</v>
+      </c>
+      <c r="C10" s="9">
         <v>0</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>200</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>60</v>
       </c>
-      <c r="E10" s="8">
+      <c r="F10" s="8">
         <v>5</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>0.5</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H10" s="8">
         <f t="shared" si="0"/>
         <v>7.03125</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <f t="shared" si="1"/>
         <v>0.1171875</v>
       </c>
-      <c r="I10" s="9">
+      <c r="J10" s="9">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="J10" s="9">
+      <c r="K10" s="9">
         <f t="shared" si="3"/>
         <v>2840</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="9">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9">
         <v>0</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>200</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>40</v>
       </c>
-      <c r="E11" s="8">
+      <c r="F11" s="8">
         <v>10</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="10">
+      <c r="I11" s="10">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="I11" s="9">
+      <c r="J11" s="9">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="J11" s="9">
+      <c r="K11" s="9">
         <f t="shared" si="3"/>
         <v>3080</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2747,7 +2836,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2760,14 +2849,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2883,7 +2972,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2892,7 +2981,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2903,14 +2992,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2934,53 +3023,53 @@
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="9">
         <v>0.2</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="9">
         <v>100</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="9">
         <v>0.5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="9">
         <v>80</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="9">
         <v>0.3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3104,5 +3193,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish introduction and each airdrop part
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A916F3E-9AAD-481B-8524-E8536AA7249D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DE9EB9-3F5F-4B01-9965-94203B68F422}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="134">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -533,6 +533,34 @@
   </si>
   <si>
     <t>散角参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二倍镜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_TIMES_SCOPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四倍镜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>八倍镜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4_TIMES_SCOPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8_TIMES_SCOPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增大视距减小视角</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -652,35 +680,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -980,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C52A79-B566-4FC5-8948-3AF6DCA12DD3}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -995,478 +1016,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>9999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>30</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>30</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <f>IF(ISBLANK(B4),"",A3+1)</f>
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>80</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2.5</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>4</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>25</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>100</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <f t="shared" ref="A5:A15" si="0">IF(ISBLANK(B5),"",A4+1)</f>
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>20</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>100</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>2.5</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>25</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>50</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>150</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>1.5</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>30</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>50</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>150</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>40</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>35</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>50</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>100</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>40</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>20</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>600</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.5</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>8</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>100</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>20</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>0.3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>10</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>150</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>10</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>20</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>60</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>50</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>30</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>10</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>100</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>6</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>30</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>25</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="str">
+      <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1482,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF40BAA-8A38-4EF9-A863-ECFFAD2B3CB6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1493,296 +1514,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <f>COUNT(武器!A3:A25)</f>
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>0.15</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>50</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <f>IF(ISBLANK(B4),"",A3+1)</f>
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>150</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>0.25</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>25</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <f t="shared" ref="A5:A8" si="0">IF(ISBLANK(B5),"",A4+1)</f>
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>0.3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>0.5</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="str">
+      <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1799,7 +1820,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1813,371 +1834,407 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <f>COUNT(防具!A3:A10) + COUNT(武器!A3:A20)</f>
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <f>IF(ISBLANK(B4),"",A3+1)</f>
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>-20</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>60</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <f t="shared" ref="A5:A13" si="0">IF(ISBLANK(B5),"",A4+1)</f>
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>-100</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>8</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="str">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="str">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="str">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2193,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2212,184 +2269,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>120</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
+        <v>160</v>
+      </c>
+      <c r="F3" s="2">
+        <v>124</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>160</v>
+      </c>
+      <c r="F4" s="2">
+        <v>124</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>90</v>
+      </c>
+      <c r="E5" s="3">
+        <v>160</v>
+      </c>
+      <c r="F5" s="2">
+        <v>124</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>80</v>
+      </c>
+      <c r="E6" s="3">
         <v>200</v>
       </c>
-      <c r="F3" s="9">
-        <v>124</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="F6" s="2">
+        <v>115</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5">
-        <v>100</v>
-      </c>
-      <c r="E4" s="5">
-        <v>200</v>
-      </c>
-      <c r="F4" s="9">
-        <v>124</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="3">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5">
-        <v>90</v>
-      </c>
-      <c r="E5" s="5">
-        <v>200</v>
-      </c>
-      <c r="F5" s="9">
-        <v>124</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0.43</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5">
-        <v>80</v>
-      </c>
-      <c r="E6" s="5">
-        <v>250</v>
-      </c>
-      <c r="F6" s="9">
-        <v>115</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>1.5</v>
       </c>
-      <c r="K6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2405,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2421,402 +2473,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="2">
         <v>1000</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="2">
         <v>200</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>200</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>200</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>0.5</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.75</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <f>1000 * G3</f>
         <v>750</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <f>(1000-H3)/E3</f>
         <v>1.25</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="2">
         <f>(C3+D3+E3)</f>
         <v>600</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="2">
         <f>J3</f>
         <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="2">
         <v>500</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>200</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>180</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>0.75</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0.6</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <f>H3*G4</f>
         <v>450</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="7">
         <f>(H3-H4)/E4</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="2">
         <f>(D4+E4)</f>
         <v>380</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="2">
         <f>J4+K3</f>
         <v>980</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="2">
         <v>250</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>160</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>0.5</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <f t="shared" ref="H5:H11" si="0">H4*G5</f>
         <v>225</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <f t="shared" ref="I5:I11" si="1">(H4-H5)/E5</f>
         <v>1.40625</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="2">
         <f t="shared" ref="J5:J11" si="2">(D5+E5)</f>
         <v>360</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="2">
         <f t="shared" ref="K5:K11" si="3">J5+K4</f>
         <v>1340</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="2">
         <v>125</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="2">
         <v>0</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>200</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>140</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>1.25</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>0.5</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <f t="shared" si="1"/>
         <v>0.8035714285714286</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="2">
         <f t="shared" si="2"/>
         <v>340</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="2">
         <f t="shared" si="3"/>
         <v>1680</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
-        <v>63</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="2">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>200</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>120</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>1.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.5</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <f t="shared" si="0"/>
         <v>56.25</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="2">
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="2">
         <v>50</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="2">
         <v>0</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>200</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>100</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>0.5</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <f t="shared" si="1"/>
         <v>0.28125</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="2">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="2">
         <f t="shared" si="3"/>
         <v>2300</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="2">
         <v>50</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>200</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>80</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>0.5</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <f t="shared" si="0"/>
         <v>14.0625</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="2">
         <f t="shared" si="2"/>
         <v>280</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="2">
         <f t="shared" si="3"/>
         <v>2580</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="2">
         <v>50</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="2">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>200</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>60</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>0.5</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <f t="shared" si="0"/>
         <v>7.03125</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <f t="shared" si="1"/>
         <v>0.1171875</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="2">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="2">
         <f t="shared" si="3"/>
         <v>2840</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="2">
         <v>50</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="2">
         <v>0</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>200</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>40</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>10</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="2">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
         <v>3080</v>
       </c>
@@ -2835,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22578DC-6594-4E6E-A10D-A4570B4B155F}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2849,122 +2901,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="2">
         <v>500</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="2">
         <v>3000</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="2">
         <v>50</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="2">
         <v>100</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="2">
         <v>300</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="2">
         <v>200</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="2">
         <v>600</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2980,8 +3032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F563B68-9CCD-4F9C-A882-9CF58895B09C}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2992,200 +3044,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="2">
         <v>0.2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="2">
         <v>100</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="2">
         <v>0.5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="2">
         <v>80</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="2">
         <v>0.3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix macro name bug
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DE9EB9-3F5F-4B01-9965-94203B68F422}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507FCD9-AA14-43B9-A5DF-E8C10B791C73}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -540,10 +540,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2_TIMES_SCOPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>四倍镜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -552,15 +548,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4_TIMES_SCOPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8_TIMES_SCOPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>增大视距减小视角</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCOPE_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCOPE_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCOPE_8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C52A79-B566-4FC5-8948-3AF6DCA12DD3}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1503,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF40BAA-8A38-4EF9-A863-ECFFAD2B3CB6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1988,7 +1988,7 @@
         <v>127</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>90</v>
@@ -2003,7 +2003,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2012,10 +2012,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>90</v>
@@ -2030,7 +2030,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2039,10 +2039,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>90</v>
@@ -2057,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2457,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2887,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22578DC-6594-4E6E-A10D-A4570B4B155F}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3032,8 +3032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F563B68-9CCD-4F9C-A882-9CF58895B09C}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finish score system and communication with backend
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D52BCA8-13C1-426E-A64D-3566A5664BD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BCEF7E-0FA0-4F43-95A1-AACB74CF079D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="168">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -562,6 +562,126 @@
   <si>
     <t>SCOPE_8</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀得分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀一个对手获得分数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分14</t>
+  </si>
+  <si>
+    <t>得分15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>得分16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第1名得分</t>
+  </si>
+  <si>
+    <t>第2名得分</t>
+  </si>
+  <si>
+    <t>第3名得分</t>
+  </si>
+  <si>
+    <t>第4名得分</t>
+  </si>
+  <si>
+    <t>第5名得分</t>
+  </si>
+  <si>
+    <t>第6名得分</t>
+  </si>
+  <si>
+    <t>第7名得分</t>
+  </si>
+  <si>
+    <t>第8名得分</t>
+  </si>
+  <si>
+    <t>第9名得分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第10名得分</t>
+  </si>
+  <si>
+    <t>第11名得分</t>
+  </si>
+  <si>
+    <t>第12名得分</t>
+  </si>
+  <si>
+    <t>第13名得分</t>
+  </si>
+  <si>
+    <t>第14名得分</t>
+  </si>
+  <si>
+    <t>第15名得分</t>
+  </si>
+  <si>
+    <t>第16名得分</t>
   </si>
 </sst>
 </file>
@@ -694,7 +814,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -718,6 +837,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,18 +1138,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1514,16 +1636,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1565,7 +1687,7 @@
       <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.15</v>
       </c>
       <c r="F3" s="2">
@@ -1592,7 +1714,7 @@
       <c r="D4" s="2">
         <v>150</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.25</v>
       </c>
       <c r="F4" s="2">
@@ -1619,7 +1741,7 @@
       <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.3</v>
       </c>
       <c r="F5" s="2">
@@ -1646,7 +1768,7 @@
       <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.5</v>
       </c>
       <c r="F6" s="2">
@@ -1667,7 +1789,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1680,7 +1802,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1834,16 +1956,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2250,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -2269,18 +2391,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2334,7 +2456,7 @@
       <c r="F3" s="2">
         <v>124</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>0.5</v>
       </c>
       <c r="H3" s="2">
@@ -2473,19 +2595,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2538,17 +2660,17 @@
       <c r="E3" s="2">
         <v>200</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0.5</v>
       </c>
       <c r="G3" s="2">
         <v>0.75</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>1000 * G3</f>
         <v>750</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <f>(1000-H3)/E3</f>
         <v>1.25</v>
       </c>
@@ -2577,17 +2699,17 @@
       <c r="E4" s="2">
         <v>180</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0.75</v>
       </c>
       <c r="G4" s="2">
         <v>0.6</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f>H3*G4</f>
         <v>450</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <f>(H3-H4)/E4</f>
         <v>1.6666666666666667</v>
       </c>
@@ -2616,17 +2738,17 @@
       <c r="E5" s="2">
         <v>160</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="2">
         <v>0.5</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" ref="H5:H11" si="0">H4*G5</f>
         <v>225</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <f t="shared" ref="I5:I11" si="1">(H4-H5)/E5</f>
         <v>1.40625</v>
       </c>
@@ -2655,17 +2777,17 @@
       <c r="E6" s="2">
         <v>140</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1.25</v>
       </c>
       <c r="G6" s="2">
         <v>0.5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f t="shared" si="1"/>
         <v>0.8035714285714286</v>
       </c>
@@ -2694,17 +2816,17 @@
       <c r="E7" s="2">
         <v>120</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1.5</v>
       </c>
       <c r="G7" s="2">
         <v>0.5</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
         <v>56.25</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
@@ -2733,17 +2855,17 @@
       <c r="E8" s="2">
         <v>100</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>0.5</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <f t="shared" si="1"/>
         <v>0.28125</v>
       </c>
@@ -2772,17 +2894,17 @@
       <c r="E9" s="2">
         <v>80</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>3</v>
       </c>
       <c r="G9" s="2">
         <v>0.5</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
         <v>14.0625</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
@@ -2811,17 +2933,17 @@
       <c r="E10" s="2">
         <v>60</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="2">
         <v>0.5</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>7.03125</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
         <v>0.1171875</v>
       </c>
@@ -2850,17 +2972,17 @@
       <c r="E11" s="2">
         <v>40</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>10</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
@@ -2901,14 +3023,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3032,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F563B68-9CCD-4F9C-A882-9CF58895B09C}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3044,14 +3166,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3123,121 +3245,223 @@
       <c r="C5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="2">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="2">
+        <v>400</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="2">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="2">
+        <v>300</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="3">
+        <v>60</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="2">
+        <v>250</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="2">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="2">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="2">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="2">
+        <v>150</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="2">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="2">
+        <v>100</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="2">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="2">
+        <v>90</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="A13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="2">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix armor bug, update player sheet
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD91927-6085-470C-9C82-D18600FFC45B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBB4A5-A568-4EAB-8A07-D8A370CFE30D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,10 +416,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最大减伤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>密码箱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -705,6 +701,10 @@
   </si>
   <si>
     <t>玩家拾取物品的最大距离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大减伤比</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -847,8 +847,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -862,8 +862,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,7 +1192,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
@@ -1212,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D3" s="2">
         <v>9999</v>
@@ -1460,10 +1460,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D11" s="2">
         <v>20</v>
@@ -1491,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="2">
         <v>10</v>
@@ -1515,7 +1515,7 @@
         <v>25</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1656,6 +1656,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1685,11 +1686,9 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1711,7 +1710,7 @@
       <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="13">
         <v>0.15</v>
       </c>
       <c r="F3" s="2">
@@ -1738,7 +1737,7 @@
       <c r="D4" s="2">
         <v>150</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="13">
         <v>0.25</v>
       </c>
       <c r="F4" s="2">
@@ -1765,7 +1764,7 @@
       <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="13">
         <v>0.3</v>
       </c>
       <c r="F5" s="2">
@@ -1784,15 +1783,15 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="13">
         <v>0.5</v>
       </c>
       <c r="F6" s="2">
@@ -1802,7 +1801,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1813,7 +1812,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1826,7 +1825,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2008,7 +2007,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>37</v>
@@ -2104,13 +2103,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -2122,7 +2121,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2131,10 +2130,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>90</v>
@@ -2149,7 +2148,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2158,10 +2157,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>90</v>
@@ -2176,7 +2175,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2185,10 +2184,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>90</v>
@@ -2203,7 +2202,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2638,7 +2637,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>49</v>
@@ -3193,7 +3192,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -3206,7 +3205,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -3215,7 +3214,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
@@ -3223,253 +3222,253 @@
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="2">
         <v>0.2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2">
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" s="2">
         <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="2">
         <v>0.3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="2">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="2">
         <v>400</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2">
         <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="2">
         <v>300</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E7" s="3">
         <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2">
         <v>250</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="2">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="2">
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="2">
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="2">
         <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" s="2">
         <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="2">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="2">
         <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" s="2">
         <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14" s="2">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -3508,12 +3507,12 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add param for scopes to check
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBB4A5-A568-4EAB-8A07-D8A370CFE30D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B69C8D3-CCBF-47D5-B35D-DE6F0CC3E7EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="175">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -520,10 +520,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>只能用于抵挡毒伤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>物品数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -705,6 +701,14 @@
   </si>
   <si>
     <t>最大减伤比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只能用于抵挡电场腐蚀</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -850,6 +854,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -860,9 +867,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1148,7 +1152,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1162,18 +1166,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1192,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
@@ -1650,27 +1654,27 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="21.875" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="8" max="8" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1686,9 +1690,11 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1710,7 +1716,7 @@
       <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="9">
         <v>0.15</v>
       </c>
       <c r="F3" s="2">
@@ -1737,7 +1743,7 @@
       <c r="D4" s="2">
         <v>150</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="9">
         <v>0.25</v>
       </c>
       <c r="F4" s="2">
@@ -1764,7 +1770,7 @@
       <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="9">
         <v>0.3</v>
       </c>
       <c r="F5" s="2">
@@ -1791,7 +1797,7 @@
       <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="9">
         <v>0.5</v>
       </c>
       <c r="F6" s="2">
@@ -1801,7 +1807,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,7 +1818,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1825,7 +1831,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1965,7 +1971,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1979,16 +1985,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2130,16 +2136,16 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -2148,7 +2154,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2157,16 +2163,16 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -2175,7 +2181,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2184,16 +2190,16 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -2202,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2396,7 +2402,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2414,18 +2420,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2603,7 +2609,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2618,26 +2624,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>49</v>
@@ -3033,7 +3039,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3046,14 +3052,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3178,7 +3184,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3191,14 +3197,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3271,204 +3277,204 @@
         <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" s="2">
         <v>400</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E6" s="2">
         <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2">
         <v>300</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="3">
         <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="2">
         <v>250</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="2">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="2">
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="2">
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="2">
         <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="2">
         <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" s="2">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="2">
         <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="2">
         <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E14" s="2">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>

</xml_diff>

<commit_message>
fix adjust land position bug, ensure circle center in the map
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B69C8D3-CCBF-47D5-B35D-DE6F0CC3E7EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3535B22B-E2C8-4CA0-AA39-7359FBB72F92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="179">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,10 +200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>毒圈数据表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>阶段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -709,6 +705,26 @@
   </si>
   <si>
     <t>只能用于抵挡电场腐蚀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始半径为1000，某一阶段半径=上一阶段半径*收缩比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收缩速度=(上一阶段半径-该阶段半径)/移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动指缩圈移动所用帧数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电圈数据表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -745,12 +761,24 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -828,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -867,6 +895,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1152,7 +1192,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1236,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
@@ -1216,10 +1256,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="D3" s="2">
         <v>9999</v>
@@ -1233,8 +1273,8 @@
       <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="2">
-        <v>30</v>
+      <c r="H3" s="17">
+        <v>20</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -1247,10 +1287,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -1278,10 +1318,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2">
         <v>20</v>
@@ -1309,10 +1349,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D6" s="2">
         <v>15</v>
@@ -1340,10 +1380,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -1371,10 +1411,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
@@ -1402,10 +1442,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -1433,10 +1473,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D10" s="2">
         <v>5</v>
@@ -1464,10 +1504,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D11" s="2">
         <v>20</v>
@@ -1495,10 +1535,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="2">
         <v>10</v>
@@ -1519,7 +1559,7 @@
         <v>25</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1654,7 +1694,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1690,10 +1730,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>38</v>
@@ -1735,10 +1775,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2">
         <v>150</v>
@@ -1753,7 +1793,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1762,10 +1802,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2">
         <v>200</v>
@@ -1780,7 +1820,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,10 +1829,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -1807,7 +1847,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1971,7 +2011,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2013,7 +2053,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>37</v>
@@ -2055,13 +2095,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2">
         <v>-20</v>
@@ -2073,7 +2113,7 @@
         <v>60</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2082,13 +2122,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="2">
         <v>-100</v>
@@ -2100,7 +2140,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2109,13 +2149,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -2127,7 +2167,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2136,13 +2176,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2154,7 +2194,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2163,13 +2203,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -2181,7 +2221,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2190,13 +2230,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -2208,7 +2248,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2402,7 +2442,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2454,7 +2494,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
@@ -2606,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2625,7 +2665,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2640,37 +2680,37 @@
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3024,9 +3064,83 @@
         <v>3080</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D16:J16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3039,7 +3153,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3053,7 +3167,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3066,16 +3180,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
@@ -3086,10 +3200,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2">
         <v>500</v>
@@ -3098,7 +3212,7 @@
         <v>3000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3106,10 +3220,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2">
         <v>50</v>
@@ -3118,7 +3232,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3126,10 +3240,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
@@ -3138,7 +3252,7 @@
         <v>300</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3146,10 +3260,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D6" s="2">
         <v>200</v>
@@ -3158,7 +3272,7 @@
         <v>600</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3184,7 +3298,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3198,7 +3312,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3211,7 +3325,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -3220,7 +3334,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
@@ -3228,253 +3342,253 @@
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2">
         <v>0.2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2">
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="2">
         <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="2">
         <v>0.3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E5" s="2">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="2">
         <v>400</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2">
         <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="2">
         <v>300</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E7" s="3">
         <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" s="2">
         <v>250</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" s="2">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" s="2">
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E9" s="2">
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" s="2">
         <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="2">
         <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" s="2">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="2">
         <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="2">
         <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E14" s="2">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>

</xml_diff>

<commit_message>
finish swimming part, update some parameter in sheet
</commit_message>
<xml_diff>
--- a/logic/sheet/data.xlsx
+++ b/logic/sheet/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4174B00B-66A9-4D8B-855A-016443BB6A8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130B9AF2-C6DF-406B-81C3-886337FEED08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="武器" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="196">
   <si>
     <t>职业</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -292,18 +292,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>爆炸声</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOM_SOUND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆炸物爆炸时发出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>半径</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -708,23 +696,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>初始半径为1000，某一阶段半径=上一阶段半径*收缩比</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>说明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>收缩速度=(上一阶段半径-该阶段半径)/移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动指缩圈移动所用帧数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>电圈数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相关参数说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.初始半径为1000，某一阶段半径=上一阶段半径*收缩比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.移动指缩圈移动所用帧数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.收缩速度=(上一阶段半径-该阶段半径)/移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.半径指人物碰撞半径，人物模型为圆形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.移动因数指每一次移动时的距离会在基本距离的基础上乘以该因子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.技能因数中医疗兵指医疗兵对其他人治疗效果打的折扣，信号兵指一回合通信上限，狙击手指狙击枪伤害倍数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.耐久度会进入减伤结算公式，拾取相同防具耐久度会像弹药一样线性增加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.最大减伤比指该防具耐久度趋于无穷大时的减伤比例，实际上不可能达到</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.参数为缺省值，暂时无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.防具耐久的减少为该护甲为玩家减少的伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.不同防具减伤线性叠加而非几何叠加，假设各防具耐久均为无穷大，那么实际减伤为15%+25%+30%=70%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.耐久度相等于子弹数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.攻击距离指最大距离，但如果视距小于攻击距离，那么实际攻击距离为视距</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.出现是未归一化的刷出概率，或者说刷新物品随机数的相对权重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.伤害随弹道中心偏移玩家中心的距离高斯衰减，因此散角虽大但是远处的大散角击中伤害可以忽略</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅水移速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家在浅水移动速度系数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.消声器的参数指声音传播距离系数，绷带和急救箱指治疗值，倍镜指放大倍数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.绷带和急救箱使用时被当做武器，和武器共享攻击CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.倍镜是消耗品，遵循后覆盖前的原则</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,7 +829,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -782,12 +850,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -858,11 +932,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -894,24 +1048,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,7 +1055,100 @@
     <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1204,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C52A79-B566-4FC5-8948-3AF6DCA12DD3}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1219,18 +1448,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1249,7 +1478,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
@@ -1269,10 +1498,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D3" s="2">
         <v>9999</v>
@@ -1286,7 +1515,7 @@
       <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="11">
         <v>20</v>
       </c>
       <c r="I3" s="2">
@@ -1300,10 +1529,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -1331,10 +1560,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2">
         <v>20</v>
@@ -1362,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2">
         <v>15</v>
@@ -1393,10 +1622,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -1424,10 +1653,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
@@ -1455,10 +1684,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -1486,10 +1715,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2">
         <v>5</v>
@@ -1517,10 +1746,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2">
         <v>20</v>
@@ -1548,10 +1777,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2">
         <v>10</v>
@@ -1572,7 +1801,7 @@
         <v>25</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1606,19 +1835,19 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="str">
+      <c r="A15" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
@@ -1633,68 +1862,83 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="A17" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
     </row>
     <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="A18" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="A19" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="A20" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="A21" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="A21:J21"/>
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A20:J20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1706,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF40BAA-8A38-4EF9-A863-ECFFAD2B3CB6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1718,16 +1962,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1743,10 +1987,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>38</v>
@@ -1778,7 +2022,7 @@
       <c r="G3" s="2">
         <v>50</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1788,10 +2032,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2">
         <v>150</v>
@@ -1806,7 +2050,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1815,10 +2059,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2">
         <v>200</v>
@@ -1833,7 +2077,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1842,10 +2086,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -1860,7 +2104,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1910,64 +2154,76 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="A12" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="A15" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="A16" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
@@ -2010,8 +2266,14 @@
       <c r="H20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A16:H16"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2023,8 +2285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74A35FB-70A1-4854-8376-A9BDA6B66FB9}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2038,16 +2300,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2066,7 +2328,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>37</v>
@@ -2098,7 +2360,7 @@
       <c r="G3" s="2">
         <v>10</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2108,13 +2370,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E4" s="2">
         <v>-20</v>
@@ -2126,7 +2388,7 @@
         <v>60</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2135,13 +2397,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E5" s="2">
         <v>-100</v>
@@ -2153,7 +2415,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2162,13 +2424,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -2180,7 +2442,7 @@
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2189,13 +2451,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2207,7 +2469,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2216,13 +2478,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -2234,7 +2496,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2243,13 +2505,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -2261,7 +2523,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2291,69 +2553,78 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="str">
+      <c r="A12" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="str">
+      <c r="A13" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="A15" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="A16" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="A17" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -2441,8 +2712,12 @@
       <c r="H26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2452,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2473,18 +2748,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2507,7 +2782,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
@@ -2541,7 +2816,7 @@
       <c r="G3" s="7">
         <v>0.5</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="11">
         <v>1.8</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -2579,7 +2854,7 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="11">
         <v>5</v>
       </c>
     </row>
@@ -2625,8 +2900,8 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
-        <v>80</v>
+      <c r="D6" s="18">
+        <v>90</v>
       </c>
       <c r="E6" s="3">
         <v>200</v>
@@ -2647,9 +2922,69 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2659,10 +2994,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41FB68-2421-4E85-B599-0C1DD2C30924}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2677,26 +3012,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="A1" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>48</v>
@@ -2748,7 +3083,7 @@
       <c r="G3" s="2">
         <v>0.75</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="13">
         <f>1000 * G3</f>
         <v>750</v>
       </c>
@@ -2970,8 +3305,8 @@
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="2">
-        <v>200</v>
+      <c r="D9" s="45">
+        <v>150</v>
       </c>
       <c r="E9" s="2">
         <v>80</v>
@@ -2990,13 +3325,13 @@
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="45">
         <f t="shared" si="2"/>
-        <v>280</v>
-      </c>
-      <c r="K9" s="2">
+        <v>230</v>
+      </c>
+      <c r="K9" s="45">
         <f t="shared" si="3"/>
-        <v>2580</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3009,8 +3344,8 @@
       <c r="C10" s="2">
         <v>0</v>
       </c>
-      <c r="D10" s="2">
-        <v>200</v>
+      <c r="D10" s="45">
+        <v>100</v>
       </c>
       <c r="E10" s="2">
         <v>60</v>
@@ -3029,13 +3364,13 @@
         <f t="shared" si="1"/>
         <v>0.1171875</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="45">
         <f t="shared" si="2"/>
-        <v>260</v>
-      </c>
-      <c r="K10" s="2">
+        <v>160</v>
+      </c>
+      <c r="K10" s="45">
         <f t="shared" si="3"/>
-        <v>2840</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3048,8 +3383,8 @@
       <c r="C11" s="2">
         <v>0</v>
       </c>
-      <c r="D11" s="2">
-        <v>200</v>
+      <c r="D11" s="45">
+        <v>100</v>
       </c>
       <c r="E11" s="2">
         <v>40</v>
@@ -3068,13 +3403,13 @@
         <f t="shared" si="1"/>
         <v>0.17578125</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="45">
         <f t="shared" si="2"/>
-        <v>240</v>
-      </c>
-      <c r="K11" s="2">
+        <v>140</v>
+      </c>
+      <c r="K11" s="45">
         <f t="shared" si="3"/>
-        <v>3080</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3082,78 +3417,77 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="A14" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="A15" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="16" t="s">
+      <c r="A16" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A17:K17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3163,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22578DC-6594-4E6E-A10D-A4570B4B155F}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3179,14 +3513,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3227,7 +3561,7 @@
       <c r="F3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -3270,32 +3604,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="2">
-        <v>200</v>
-      </c>
-      <c r="E6" s="2">
-        <v>600</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3311,8 +3625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F563B68-9CCD-4F9C-A882-9CF58895B09C}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3325,21 +3639,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -3348,7 +3662,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
@@ -3356,258 +3670,264 @@
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B3" s="2">
         <v>0.2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2">
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E4" s="2">
         <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" s="2">
         <v>0.3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E5" s="2">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2">
         <v>400</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E6" s="2">
         <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" s="2">
         <v>300</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E7" s="3">
         <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2">
         <v>250</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E8" s="2">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" s="2">
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2">
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2">
         <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="2">
         <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E11" s="2">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B12" s="2">
         <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" s="2">
         <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E14" s="2">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>

</xml_diff>